<commit_message>
Edited the projected cost doc for mech components with accurate values
</commit_message>
<xml_diff>
--- a/ToasterChargerModule/Toaster Charger #2/Projected Cost of Charger.xlsx
+++ b/ToasterChargerModule/Toaster Charger #2/Projected Cost of Charger.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sujayt123\Documents\GitHub\rone-electrical\ToasterChargerModule\Toaster Charger #2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21268" windowHeight="8474"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20640" windowHeight="8475"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Cost</t>
   </si>
@@ -102,6 +97,18 @@
   </si>
   <si>
     <t>RHM11.8KCFCT-ND (Rset)</t>
+  </si>
+  <si>
+    <t>http://www.omnicase.com/</t>
+  </si>
+  <si>
+    <t>https://www.bigbluesaw.com/</t>
+  </si>
+  <si>
+    <t>http://goo.gl/Xpt3aH</t>
+  </si>
+  <si>
+    <t>in lab</t>
   </si>
 </sst>
 </file>
@@ -172,6 +179,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -188,7 +263,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="535353"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -226,7 +301,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -261,7 +336,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -438,7 +513,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -449,21 +524,21 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.8984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.3984375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.796875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.796875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.796875" style="1"/>
+    <col min="1" max="1" width="27.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
@@ -477,12 +552,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -500,7 +575,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -518,7 +593,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -536,7 +611,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -554,7 +629,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -572,7 +647,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -590,7 +665,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -608,7 +683,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -626,18 +701,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D12" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -651,38 +726,49 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F14" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="1">
-        <v>10</v>
+        <f>348/150</f>
+        <v>2.3199999999999998</v>
       </c>
       <c r="C15" s="1">
         <v>12</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>27.839999999999996</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="1">
-        <v>0.25</v>
+        <f>12.95/50</f>
+        <v>0.25900000000000001</v>
       </c>
       <c r="C16" s="1">
         <v>8</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2.0720000000000001</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -696,27 +782,35 @@
         <f t="shared" si="0"/>
         <v>2.4000000000000004</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F17" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D18" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D19" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D20" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F14" r:id="rId1"/>
+    <hyperlink ref="F15" r:id="rId2"/>
+    <hyperlink ref="F16" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added 3d body to new components. Added appropriate part for C_out. Board should be done; need to export to gerber files and get quotes.
</commit_message>
<xml_diff>
--- a/ToasterChargerModule/Toaster Charger #2/Projected Cost of Charger.xlsx
+++ b/ToasterChargerModule/Toaster Charger #2/Projected Cost of Charger.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sujayt123\Documents\GitHub\rone-electrical\ToasterChargerModule\Toaster Charger #2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20640" windowHeight="8475"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20636" windowHeight="8474"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Cost</t>
   </si>
@@ -109,6 +114,15 @@
   </si>
   <si>
     <t>in lab</t>
+  </si>
+  <si>
+    <t>http://goo.gl/rrNymK</t>
+  </si>
+  <si>
+    <t>EEUFC1V331 (Cout)</t>
+  </si>
+  <si>
+    <t>Board Options</t>
   </si>
 </sst>
 </file>
@@ -179,74 +193,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -263,7 +209,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="535353"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -513,7 +459,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -521,24 +467,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="27.3984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.8984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.3984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.3984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.8984375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.8984375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.8984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
@@ -552,12 +498,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -568,14 +514,14 @@
         <v>1</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D20" si="0">SUM(B3*C3,0)</f>
+        <f t="shared" ref="D3:D23" si="0">SUM(B3*C3,0)</f>
         <v>25</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -593,7 +539,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -611,7 +557,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -629,7 +575,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -647,7 +593,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -665,7 +611,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -683,7 +629,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -701,18 +647,30 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D12" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.53</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -730,7 +688,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -749,7 +707,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -768,7 +726,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -786,20 +744,37 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D18" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D19" s="1">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D20" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D20" s="1">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D23" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
2 layer board and new projected costs. More organization in the subdirectories now
</commit_message>
<xml_diff>
--- a/ToasterChargerModule/Toaster Charger #2/Projected Cost of Charger.xlsx
+++ b/ToasterChargerModule/Toaster Charger #2/Projected Cost of Charger.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Cost</t>
   </si>
@@ -128,9 +128,6 @@
     <t>(Assuming quotes are correct)</t>
   </si>
   <si>
-    <t>4 days</t>
-  </si>
-  <si>
     <t>Advanced Circuits (standard specs, w/the works):</t>
   </si>
   <si>
@@ -138,6 +135,12 @@
   </si>
   <si>
     <t>per board, 2nd pcb option</t>
+  </si>
+  <si>
+    <t>3 layers: 4 days</t>
+  </si>
+  <si>
+    <t>2 layers: 3 days</t>
   </si>
 </sst>
 </file>
@@ -482,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -529,7 +532,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D23" si="0">SUM(B3*C3,0)</f>
+        <f t="shared" ref="D3:D18" si="0">SUM(B3*C3,0)</f>
         <v>25</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -775,51 +778,81 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B21" s="1">
-        <v>776.64</v>
+        <v>189.63</v>
       </c>
       <c r="C21" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="0"/>
-        <v>776.64</v>
+        <f>SUM(B21*C21,0)</f>
+        <v>948.15</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B22" s="1">
-        <v>434.66</v>
+        <v>111.58</v>
       </c>
       <c r="C22" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="0"/>
-        <v>869.32</v>
+        <f>SUM(B22*C22,0)</f>
+        <v>1115.8</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D25" s="2" t="s">
+      <c r="A25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="1">
+        <v>101.65</v>
+      </c>
+      <c r="C25" s="1">
+        <v>5</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" ref="D25:D26" si="1">SUM(B25*C25,0)</f>
+        <v>508.25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="1">
+        <v>58.58</v>
+      </c>
+      <c r="C26" s="1">
+        <v>10</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="1"/>
+        <v>585.79999999999995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D32" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D33" s="1">
+        <f>SUM(D3:D20,B26)</f>
+        <v>219.30200000000002</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D26" s="1">
-        <f>SUM(D3:D20,D22/2)</f>
-        <v>595.38200000000006</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Thermal vias, thermal connections, parts repositioned, new LED component.
</commit_message>
<xml_diff>
--- a/ToasterChargerModule/Toaster Charger #2/Projected Cost of Charger.xlsx
+++ b/ToasterChargerModule/Toaster Charger #2/Projected Cost of Charger.xlsx
@@ -116,12 +116,6 @@
     <t>in lab</t>
   </si>
   <si>
-    <t>http://goo.gl/rrNymK</t>
-  </si>
-  <si>
-    <t>EEUFC1V331 (Cout)</t>
-  </si>
-  <si>
     <t>Board Options</t>
   </si>
   <si>
@@ -141,6 +135,12 @@
   </si>
   <si>
     <t>2 layers: 3 days</t>
+  </si>
+  <si>
+    <t>http://goo.gl/3D2k0X</t>
+  </si>
+  <si>
+    <t>ECA-1VM331</t>
   </si>
 </sst>
 </file>
@@ -487,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -667,20 +667,20 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B11" s="1">
-        <v>0.53</v>
+        <v>0.41</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>0.53</v>
+        <v>0.41</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -770,20 +770,20 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B21" s="1">
         <v>189.63</v>
@@ -798,7 +798,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B22" s="1">
         <v>111.58</v>
@@ -813,7 +813,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B25" s="1">
         <v>101.65</v>
@@ -828,7 +828,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B26" s="1">
         <v>58.58</v>
@@ -843,16 +843,16 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D32" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D33" s="1">
         <f>SUM(D3:D20,B26)</f>
-        <v>219.30200000000002</v>
+        <v>219.18200000000002</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>